<commit_message>
CREATE OR ALTER PROCEDURE inserciones.TestInsertarEmpleados OK
</commit_message>
<xml_diff>
--- a/test-caso2-insert.xlsx
+++ b/test-caso2-insert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\ddbba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EC0E55-8776-4B72-8CCF-3DE74A877029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679DD635-A236-4C03-BBB0-0F1858C63462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="2910" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
+    <workbookView xWindow="5310" yWindow="3600" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
   </bookViews>
   <sheets>
     <sheet name="sucursal" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="297">
   <si>
     <t>Ciudad</t>
   </si>
@@ -1102,7 +1102,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="16">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1306,6 +1306,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1313,15 +1322,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1337,22 +1337,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1378,7 +1362,7 @@
     <tableColumn id="1" xr3:uid="{B279F2FA-3A4D-477B-A0B7-5526FBA1CE34}" name="Ciudad"/>
     <tableColumn id="2" xr3:uid="{BF06278C-AB08-44C6-8E5B-FA0847539AD1}" name="Reemplazar por"/>
     <tableColumn id="3" xr3:uid="{9516CA9C-D27E-4565-9721-89106345AB3C}" name="direccion"/>
-    <tableColumn id="4" xr3:uid="{05C2561D-F0B8-40BE-976B-467B9FE3ACE5}" name="Horario" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{05C2561D-F0B8-40BE-976B-467B9FE3ACE5}" name="Horario" dataDxfId="15"/>
     <tableColumn id="5" xr3:uid="{CADF9AC2-BE7B-44DF-8828-6D257CD1937F}" name="Telefono"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1386,7 +1370,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91E7DD32-2B6F-4C6F-9B16-BBA140E5DC35}" name="Tabla2" displayName="Tabla2" ref="A2:K19" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91E7DD32-2B6F-4C6F-9B16-BBA140E5DC35}" name="Tabla2" displayName="Tabla2" ref="A2:K19" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A2:K19" xr:uid="{91E7DD32-2B6F-4C6F-9B16-BBA140E5DC35}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{411F086D-095A-47E3-AE29-CED45684D248}" name="Legajo/ID" dataDxfId="10"/>
@@ -1831,7 +1815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D04809A-CB1B-4D46-A903-714B4EC2DF94}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+    <sheetView topLeftCell="F4" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -2463,10 +2447,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D68890E-1A4A-4BA5-B83B-61727FCC66D7}">
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2501,6 +2485,14 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3760,12 +3752,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3980,19 +3973,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{652FEED1-E158-4EC5-B971-D1B087C7E1CB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E17D9C7C-79F5-4A33-AEBC-02D7C68BFB0C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4017,11 +4011,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E17D9C7C-79F5-4A33-AEBC-02D7C68BFB0C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{652FEED1-E158-4EC5-B971-D1B087C7E1CB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "CREATE OR ALTER PROCEDURE inserciones.TestInsertarEmpleados OK"
This reverts commit 574b13afb2f95a71cbc1ee6f642ceb7e3767d093.
</commit_message>
<xml_diff>
--- a/test-caso2-insert.xlsx
+++ b/test-caso2-insert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\ddbba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679DD635-A236-4C03-BBB0-0F1858C63462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EC0E55-8776-4B72-8CCF-3DE74A877029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="3600" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
+    <workbookView xWindow="4620" yWindow="2910" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
   </bookViews>
   <sheets>
     <sheet name="sucursal" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="297">
   <si>
     <t>Ciudad</t>
   </si>
@@ -1102,7 +1102,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1306,15 +1306,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1322,6 +1313,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1337,6 +1337,22 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1362,7 +1378,7 @@
     <tableColumn id="1" xr3:uid="{B279F2FA-3A4D-477B-A0B7-5526FBA1CE34}" name="Ciudad"/>
     <tableColumn id="2" xr3:uid="{BF06278C-AB08-44C6-8E5B-FA0847539AD1}" name="Reemplazar por"/>
     <tableColumn id="3" xr3:uid="{9516CA9C-D27E-4565-9721-89106345AB3C}" name="direccion"/>
-    <tableColumn id="4" xr3:uid="{05C2561D-F0B8-40BE-976B-467B9FE3ACE5}" name="Horario" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{05C2561D-F0B8-40BE-976B-467B9FE3ACE5}" name="Horario" dataDxfId="16"/>
     <tableColumn id="5" xr3:uid="{CADF9AC2-BE7B-44DF-8828-6D257CD1937F}" name="Telefono"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1370,7 +1386,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91E7DD32-2B6F-4C6F-9B16-BBA140E5DC35}" name="Tabla2" displayName="Tabla2" ref="A2:K19" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91E7DD32-2B6F-4C6F-9B16-BBA140E5DC35}" name="Tabla2" displayName="Tabla2" ref="A2:K19" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
   <autoFilter ref="A2:K19" xr:uid="{91E7DD32-2B6F-4C6F-9B16-BBA140E5DC35}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{411F086D-095A-47E3-AE29-CED45684D248}" name="Legajo/ID" dataDxfId="10"/>
@@ -1815,7 +1831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D04809A-CB1B-4D46-A903-714B4EC2DF94}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -2447,10 +2463,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D68890E-1A4A-4BA5-B83B-61727FCC66D7}">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2485,14 +2501,6 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3752,13 +3760,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3973,20 +3980,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E17D9C7C-79F5-4A33-AEBC-02D7C68BFB0C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{652FEED1-E158-4EC5-B971-D1B087C7E1CB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4011,9 +4017,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{652FEED1-E158-4EC5-B971-D1B087C7E1CB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E17D9C7C-79F5-4A33-AEBC-02D7C68BFB0C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
error: case 1 - sp productos
</commit_message>
<xml_diff>
--- a/test-caso2-insert.xlsx
+++ b/test-caso2-insert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\ddbba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EC0E55-8776-4B72-8CCF-3DE74A877029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B977A428-EAB8-4FFA-9493-C5DD7AC0090C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="2910" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
+    <workbookView xWindow="5310" yWindow="3600" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
   </bookViews>
   <sheets>
     <sheet name="sucursal" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="297">
   <si>
     <t>Ciudad</t>
   </si>
@@ -1102,7 +1102,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="16">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1306,6 +1306,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1313,15 +1322,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1337,22 +1337,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1378,7 +1362,7 @@
     <tableColumn id="1" xr3:uid="{B279F2FA-3A4D-477B-A0B7-5526FBA1CE34}" name="Ciudad"/>
     <tableColumn id="2" xr3:uid="{BF06278C-AB08-44C6-8E5B-FA0847539AD1}" name="Reemplazar por"/>
     <tableColumn id="3" xr3:uid="{9516CA9C-D27E-4565-9721-89106345AB3C}" name="direccion"/>
-    <tableColumn id="4" xr3:uid="{05C2561D-F0B8-40BE-976B-467B9FE3ACE5}" name="Horario" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{05C2561D-F0B8-40BE-976B-467B9FE3ACE5}" name="Horario" dataDxfId="15"/>
     <tableColumn id="5" xr3:uid="{CADF9AC2-BE7B-44DF-8828-6D257CD1937F}" name="Telefono"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1386,7 +1370,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91E7DD32-2B6F-4C6F-9B16-BBA140E5DC35}" name="Tabla2" displayName="Tabla2" ref="A2:K19" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91E7DD32-2B6F-4C6F-9B16-BBA140E5DC35}" name="Tabla2" displayName="Tabla2" ref="A2:K19" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A2:K19" xr:uid="{91E7DD32-2B6F-4C6F-9B16-BBA140E5DC35}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{411F086D-095A-47E3-AE29-CED45684D248}" name="Legajo/ID" dataDxfId="10"/>
@@ -1831,7 +1815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D04809A-CB1B-4D46-A903-714B4EC2DF94}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+    <sheetView topLeftCell="F4" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -2463,10 +2447,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D68890E-1A4A-4BA5-B83B-61727FCC66D7}">
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,6 +2488,22 @@
         <v>53</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2511,10 +2511,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932457C5-F4E5-40E2-86CE-923AE54F2BD9}">
-  <dimension ref="B1:C149"/>
+  <dimension ref="B1:C151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3712,6 +3712,22 @@
         <v>34</v>
       </c>
       <c r="C149" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>34</v>
+      </c>
+      <c r="C150" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>34</v>
+      </c>
+      <c r="C151" t="s">
         <v>201</v>
       </c>
     </row>
@@ -3769,6 +3785,16 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E0244CD539E758458F9751B276EDBDB5" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="940421aca186f6b6cf253ceb76bcb39c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29" xmlns:ns3="5ab81898-6d95-4a49-9528-d5d2a870eede" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f4f5da10e60c2eff5832bc3c34d166e5" ns2:_="" ns3:_="">
     <xsd:import namespace="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
@@ -3979,16 +4005,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{652FEED1-E158-4EC5-B971-D1B087C7E1CB}">
   <ds:schemaRefs>
@@ -3998,6 +4014,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E17D9C7C-79F5-4A33-AEBC-02D7C68BFB0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{664D04EC-A970-41D8-9994-316B682115F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4014,14 +4040,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E17D9C7C-79F5-4A33-AEBC-02D7C68BFB0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
CREATE OR ALTER PROCEDURE inserciones.TestInsertarProductosElectronicos
</commit_message>
<xml_diff>
--- a/test-caso2-insert.xlsx
+++ b/test-caso2-insert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\ddbba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B977A428-EAB8-4FFA-9493-C5DD7AC0090C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57550D04-FC8B-43B1-BF00-DC8AC50E4B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="3600" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
   </bookViews>
   <sheets>
     <sheet name="sucursal" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
add some cases test
</commit_message>
<xml_diff>
--- a/test-caso2-insert.xlsx
+++ b/test-caso2-insert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\ddbba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57550D04-FC8B-43B1-BF00-DC8AC50E4B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A35C9F4-0ADD-40A9-AB5C-255B12D4A2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
+    <workbookView xWindow="5310" yWindow="3600" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
   </bookViews>
   <sheets>
     <sheet name="sucursal" sheetId="1" r:id="rId1"/>
@@ -2450,7 +2450,7 @@
   <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>